<commit_message>
Refactor code structure + fix pip package issue (#9)
</commit_message>
<xml_diff>
--- a/examples/palabra/labs/lab1/lab1_result.xlsx
+++ b/examples/palabra/labs/lab1/lab1_result.xlsx
@@ -444,17 +444,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>358</t>
+          <t>348</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>192</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>156</t>
         </is>
       </c>
     </row>
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C359"/>
+  <dimension ref="A1:C349"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1896,12 +1896,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `3.0.0.2`.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -1913,12 +1913,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `3.1.0.1`.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2049,12 +2049,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `20.30.0.1`.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2627,12 +2627,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>`as2r2` does not receive any answer from `3.1.0.2`.</t>
         </is>
       </c>
     </row>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>`as2r2` does not receive any answer from `3.2.0.1`.</t>
         </is>
       </c>
     </row>
@@ -2814,12 +2814,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -2950,12 +2950,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>`as3r1` does not receive any answer from `2.0.0.2`.</t>
+          <t>OK</t>
         </is>
       </c>
     </row>
@@ -6078,12 +6078,12 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>The routing table of as1r1 have the wrong number of routes: 6, expected: 8</t>
         </is>
       </c>
     </row>
@@ -6095,12 +6095,12 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>The routing table of as1r2 have the wrong number of routes: 6, expected: 8</t>
         </is>
       </c>
     </row>
@@ -6112,12 +6112,12 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>The routing table of as2r1 have the wrong number of routes: 5, expected: 8</t>
         </is>
       </c>
     </row>
@@ -6129,12 +6129,12 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>The routing table of as2r2 have the wrong number of routes: 4, expected: 8</t>
         </is>
       </c>
     </row>
@@ -6151,7 +6151,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>The routing table of as3r1 is missing route 3.2.0.0/24</t>
+          <t>The routing table of as3r1 have the wrong number of routes: 6, expected: 9</t>
         </is>
       </c>
     </row>
@@ -6168,14 +6168,14 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>The routing table of root is missing route 0.0.0.0/0</t>
+          <t>The routing table of root have the wrong number of routes: 0, expected: 2</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Checking the routing table of root</t>
+          <t>Checking the routing table of net</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -6185,14 +6185,14 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>The routing table of root is missing route 1.1.0.0/24</t>
+          <t>The routing table of net have the wrong number of routes: 0, expected: 2</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>Checking the routing table of net</t>
+          <t>Checking the routing table of pc</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -6202,14 +6202,14 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>The routing table of net is missing route 0.0.0.0/0</t>
+          <t>The routing table of pc have the wrong number of routes: 0, expected: 2</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>Checking the routing table of net</t>
+          <t>Checking the routing table of local</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -6219,14 +6219,14 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>The routing table of net is missing route 2.1.0.0/24</t>
+          <t>The routing table of local have the wrong number of routes: 0, expected: 2</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Checking the routing table of pc</t>
+          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -6236,14 +6236,14 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>The routing table of pc is missing route 0.0.0.0/0</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>Checking the routing table of pc</t>
+          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -6253,14 +6253,14 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>The routing table of pc is missing route 3.1.0.0/24</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Checking the routing table of local</t>
+          <t>Checking on `local` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -6270,14 +6270,14 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>The routing table of local is missing route 0.0.0.0/0</t>
+          <t>named not started in the startup file of `local`</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Checking the routing table of local</t>
+          <t>Checking on `net` that `2.1.0.2` is the authority for domain `net`</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -6287,14 +6287,14 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>The routing table of local is missing route 3.2.0.0/24</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -6304,14 +6304,14 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>`resolv.conf` file not found for device `as1r1`</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -6321,14 +6321,14 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>`resolv.conf` file not found for device `as1r2`</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>Checking on `local` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -6338,14 +6338,14 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>named not started in the startup file of `local`</t>
+          <t>`resolv.conf` file not found for device `as2r1`</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>Checking on `net` that `2.1.0.2` is the authority for domain `net`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -6355,14 +6355,14 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>`resolv.conf` file not found for device `as2r2`</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -6372,14 +6372,14 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r1`</t>
+          <t>`resolv.conf` file not found for device `as3r1`</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -6389,14 +6389,14 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r2`</t>
+          <t>`resolv.conf` file not found for device `as3r2`</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `pc`</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -6406,177 +6406,7 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as2r1`</t>
-        </is>
-      </c>
-    </row>
-    <row r="350">
-      <c r="A350" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
-        </is>
-      </c>
-      <c r="B350" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C350" t="inlineStr">
-        <is>
-          <t>`resolv.conf` file not found for device `as2r2`</t>
-        </is>
-      </c>
-    </row>
-    <row r="351">
-      <c r="A351" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
-        </is>
-      </c>
-      <c r="B351" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C351" t="inlineStr">
-        <is>
-          <t>`resolv.conf` file not found for device `as3r1`</t>
-        </is>
-      </c>
-    </row>
-    <row r="352">
-      <c r="A352" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
-        </is>
-      </c>
-      <c r="B352" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C352" t="inlineStr">
-        <is>
-          <t>`resolv.conf` file not found for device `as3r2`</t>
-        </is>
-      </c>
-    </row>
-    <row r="353">
-      <c r="A353" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `pc`</t>
-        </is>
-      </c>
-      <c r="B353" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C353" t="inlineStr">
-        <is>
           <t>The local name server for device `pc` has ip `3.2.0.2`</t>
-        </is>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as1r1`</t>
-        </is>
-      </c>
-      <c r="B354" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C354" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as1r2`</t>
-        </is>
-      </c>
-      <c r="B355" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C355" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as2r1`</t>
-        </is>
-      </c>
-      <c r="B356" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C356" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as2r2`</t>
-        </is>
-      </c>
-      <c r="B357" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C357" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as3r1`</t>
-        </is>
-      </c>
-      <c r="B358" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C358" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as3r2`</t>
-        </is>
-      </c>
-      <c r="B359" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C359" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
         </is>
       </c>
     </row>
@@ -6591,7 +6421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C169"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6976,7 +6806,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -6986,14 +6816,14 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `3.0.0.2`.</t>
+          <t>`as1r2` does not receive any answer from `3.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -7003,14 +6833,14 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `3.1.0.1`.</t>
+          <t>`as1r2` does not receive any answer from `3.2.0.1`.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as1r2`</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -7020,14 +6850,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `3.1.0.2`.</t>
+          <t>`as1r2` does not receive any answer from `3.2.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -7037,14 +6867,14 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `3.2.0.1`.</t>
+          <t>`as2r1` does not receive any answer from `1.0.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as1r2`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -7054,14 +6884,14 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `3.2.0.2`.</t>
+          <t>`as2r1` does not receive any answer from `2.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `as1r2`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -7071,14 +6901,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>`as1r2` does not receive any answer from `20.30.0.1`.</t>
+          <t>`as2r1` does not receive any answer from `3.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -7088,14 +6918,14 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>`as2r1` does not receive any answer from `1.0.0.2`.</t>
+          <t>`as2r1` does not receive any answer from `3.2.0.1`.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as2r1`</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -7105,14 +6935,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>`as2r1` does not receive any answer from `2.1.0.2`.</t>
+          <t>`as2r1` does not receive any answer from `3.2.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -7122,14 +6952,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>`as2r1` does not receive any answer from `3.1.0.2`.</t>
+          <t>`as2r2` does not receive any answer from `1.0.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as2r1`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -7139,14 +6969,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>`as2r1` does not receive any answer from `3.2.0.1`.</t>
+          <t>`as2r2` does not receive any answer from `2.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as2r1`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -7156,14 +6986,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>`as2r1` does not receive any answer from `3.2.0.2`.</t>
+          <t>`as2r2` does not receive any answer from `3.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -7173,14 +7003,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>`as2r2` does not receive any answer from `1.0.0.2`.</t>
+          <t>`as2r2` does not receive any answer from `3.2.0.1`.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as2r2`</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -7190,14 +7020,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>`as2r2` does not receive any answer from `2.1.0.2`.</t>
+          <t>`as2r2` does not receive any answer from `3.2.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -7207,14 +7037,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>`as3r1` does not receive any answer from `1.0.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -7224,14 +7054,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>`as3r1` does not receive any answer from `2.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as2r2`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -7241,14 +7071,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>`as3r1` does not receive any answer from `3.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -7258,14 +7088,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>`as2r2` does not receive any answer from `3.2.0.2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `as2r2`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as3r1`</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -7282,7 +7112,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `1.0.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -7292,14 +7122,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>`as3r1` does not receive any answer from `1.0.0.2`.</t>
+          <t>`as3r2` does not receive any answer from `1.0.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `2.1.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -7309,14 +7139,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>`as3r1` does not receive any answer from `2.0.0.2`.</t>
+          <t>`as3r2` does not receive any answer from `2.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `3.1.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -7326,14 +7156,14 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>`as3r1` does not receive any answer from `2.1.0.2`.</t>
+          <t>`as3r2` does not receive any answer from `3.1.0.2`.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `3.2.0.1` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -7343,14 +7173,14 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>`as3r1` does not receive any answer from `3.1.0.2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as3r1`</t>
+          <t>Verifying `3.2.0.2` reachable from device `as3r2`</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -7367,7 +7197,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as3r1`</t>
+          <t>Verifying `1.0.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -7384,7 +7214,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `1.0.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -7394,14 +7224,14 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>`as3r2` does not receive any answer from `1.0.0.2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `1.1.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -7411,14 +7241,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>`as3r2` does not receive any answer from `2.1.0.2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `1.1.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -7428,14 +7258,14 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>`as3r2` does not receive any answer from `3.1.0.2`.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `as3r2`</t>
+          <t>Verifying `2.0.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -7452,7 +7282,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `as3r2`</t>
+          <t>Verifying `2.0.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -7469,7 +7299,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `local`</t>
+          <t>Verifying `2.1.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -7486,7 +7316,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `local`</t>
+          <t>Verifying `2.1.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -7503,7 +7333,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `local`</t>
+          <t>Verifying `3.0.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -7520,7 +7350,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `local`</t>
+          <t>Verifying `3.0.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -7537,7 +7367,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `local`</t>
+          <t>Verifying `3.1.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -7554,7 +7384,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `local`</t>
+          <t>Verifying `3.1.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -7571,7 +7401,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `local`</t>
+          <t>Verifying `3.2.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -7588,7 +7418,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `local`</t>
+          <t>Verifying `3.2.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -7605,7 +7435,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `local`</t>
+          <t>Verifying `10.20.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -7622,7 +7452,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `local`</t>
+          <t>Verifying `10.20.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -7639,7 +7469,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `local`</t>
+          <t>Verifying `10.20.1.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -7656,7 +7486,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `local`</t>
+          <t>Verifying `10.20.1.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -7673,7 +7503,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `local`</t>
+          <t>Verifying `20.30.0.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -7690,7 +7520,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `local`</t>
+          <t>Verifying `20.30.0.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -7707,7 +7537,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `local`</t>
+          <t>Verifying `20.30.1.1` reachable from device `local`</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -7724,7 +7554,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `local`</t>
+          <t>Verifying `20.30.1.2` reachable from device `local`</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -7741,7 +7571,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `local`</t>
+          <t>Verifying `1.0.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -7751,14 +7581,14 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `local`</t>
+          <t>Verifying `1.0.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -7768,14 +7598,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `local`</t>
+          <t>Verifying `1.1.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -7785,14 +7615,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `local`</t>
+          <t>Verifying `1.1.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -7802,14 +7632,14 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `local`</t>
+          <t>Verifying `2.0.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -7819,14 +7649,14 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `local`</t>
+          <t>Verifying `2.0.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -7836,14 +7666,14 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `root`</t>
+          <t>Verifying `2.1.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -7860,7 +7690,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `root`</t>
+          <t>Verifying `2.1.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -7877,7 +7707,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `root`</t>
+          <t>Verifying `3.0.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -7894,7 +7724,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `root`</t>
+          <t>Verifying `3.0.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -7911,7 +7741,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `root`</t>
+          <t>Verifying `3.1.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -7928,7 +7758,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `root`</t>
+          <t>Verifying `3.1.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -7945,7 +7775,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `root`</t>
+          <t>Verifying `3.2.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -7962,7 +7792,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `root`</t>
+          <t>Verifying `3.2.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -7979,7 +7809,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `root`</t>
+          <t>Verifying `10.20.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -7996,7 +7826,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `root`</t>
+          <t>Verifying `10.20.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -8013,7 +7843,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `root`</t>
+          <t>Verifying `10.20.1.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -8030,7 +7860,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `root`</t>
+          <t>Verifying `10.20.1.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -8047,7 +7877,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `root`</t>
+          <t>Verifying `20.30.0.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -8064,7 +7894,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `root`</t>
+          <t>Verifying `20.30.0.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -8081,7 +7911,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `root`</t>
+          <t>Verifying `20.30.1.1` reachable from device `root`</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -8098,7 +7928,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `root`</t>
+          <t>Verifying `20.30.1.2` reachable from device `root`</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -8115,7 +7945,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `root`</t>
+          <t>Verifying `1.0.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -8125,14 +7955,14 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `root`</t>
+          <t>Verifying `1.0.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -8142,14 +7972,14 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `root`</t>
+          <t>Verifying `1.1.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -8159,14 +7989,14 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `root`</t>
+          <t>Verifying `1.1.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -8176,14 +8006,14 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `root`</t>
+          <t>Verifying `2.0.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -8193,14 +8023,14 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `root`</t>
+          <t>Verifying `2.0.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -8210,14 +8040,14 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.1` reachable from device `net`</t>
+          <t>Verifying `2.1.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -8234,7 +8064,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Verifying `1.0.0.2` reachable from device `net`</t>
+          <t>Verifying `2.1.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -8251,7 +8081,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `net`</t>
+          <t>Verifying `3.0.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -8268,7 +8098,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `net`</t>
+          <t>Verifying `3.0.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -8285,7 +8115,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `net`</t>
+          <t>Verifying `3.1.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -8302,7 +8132,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `net`</t>
+          <t>Verifying `3.1.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -8319,7 +8149,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `net`</t>
+          <t>Verifying `3.2.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -8336,7 +8166,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `net`</t>
+          <t>Verifying `3.2.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -8353,7 +8183,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `net`</t>
+          <t>Verifying `10.20.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -8370,7 +8200,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `net`</t>
+          <t>Verifying `10.20.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -8387,7 +8217,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `net`</t>
+          <t>Verifying `10.20.1.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -8404,7 +8234,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `net`</t>
+          <t>Verifying `10.20.1.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -8421,7 +8251,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `net`</t>
+          <t>Verifying `20.30.0.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -8438,7 +8268,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `net`</t>
+          <t>Verifying `20.30.0.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -8455,7 +8285,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `net`</t>
+          <t>Verifying `20.30.1.1` reachable from device `net`</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -8472,7 +8302,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `net`</t>
+          <t>Verifying `20.30.1.2` reachable from device `net`</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -8489,7 +8319,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `net`</t>
+          <t>Verifying `1.1.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -8499,14 +8329,14 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `net`</t>
+          <t>Verifying `1.1.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -8516,14 +8346,14 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `net`</t>
+          <t>Verifying `2.0.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -8533,14 +8363,14 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `net`</t>
+          <t>Verifying `2.0.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -8550,14 +8380,14 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `net`</t>
+          <t>Verifying `2.1.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -8567,14 +8397,14 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `net`</t>
+          <t>Verifying `2.1.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -8584,14 +8414,14 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>ping: connect: Network is unreachable</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.1` reachable from device `pc`</t>
+          <t>Verifying `3.0.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -8608,7 +8438,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Verifying `1.1.0.2` reachable from device `pc`</t>
+          <t>Verifying `3.0.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -8625,7 +8455,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.1` reachable from device `pc`</t>
+          <t>Verifying `3.1.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -8642,7 +8472,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Verifying `2.0.0.2` reachable from device `pc`</t>
+          <t>Verifying `3.1.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -8659,7 +8489,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.1` reachable from device `pc`</t>
+          <t>Verifying `3.2.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -8676,7 +8506,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Verifying `2.1.0.2` reachable from device `pc`</t>
+          <t>Verifying `3.2.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -8693,7 +8523,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.1` reachable from device `pc`</t>
+          <t>Verifying `10.20.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -8710,7 +8540,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Verifying `3.0.0.2` reachable from device `pc`</t>
+          <t>Verifying `10.20.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -8727,7 +8557,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.1` reachable from device `pc`</t>
+          <t>Verifying `10.20.1.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -8744,7 +8574,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Verifying `3.1.0.2` reachable from device `pc`</t>
+          <t>Verifying `10.20.1.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -8761,7 +8591,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.1` reachable from device `pc`</t>
+          <t>Verifying `20.30.0.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -8778,7 +8608,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Verifying `3.2.0.2` reachable from device `pc`</t>
+          <t>Verifying `20.30.0.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -8795,7 +8625,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.1` reachable from device `pc`</t>
+          <t>Verifying `20.30.1.1` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -8812,7 +8642,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Verifying `10.20.0.2` reachable from device `pc`</t>
+          <t>Verifying `20.30.1.2` reachable from device `pc`</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -8829,7 +8659,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.1` reachable from device `pc`</t>
+          <t>Checking that named is running on device `net`</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -8839,14 +8669,14 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device net not in the network scenario.</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Verifying `10.20.1.2` reachable from device `pc`</t>
+          <t>Checking that watchfrr is not running on device `net`</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -8856,14 +8686,14 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device net not in the network scenario.</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.1` reachable from device `pc`</t>
+          <t>Checking that named is running on device `root`</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -8873,14 +8703,14 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device root not in the network scenario.</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Verifying `20.30.0.2` reachable from device `pc`</t>
+          <t>Checking that watchfrr is not running on device `root`</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -8890,14 +8720,14 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>Device root not in the network scenario.</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.1` reachable from device `pc`</t>
+          <t>as1r1 has bgp peer 1.0.0.2</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -8907,14 +8737,14 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>The peering between as1r1 and 1.0.0.2 is not up.</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Verifying `20.30.1.2` reachable from device `pc`</t>
+          <t>as1r2 has bgp peer 1.0.0.1</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -8924,14 +8754,14 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>ping: connect: Network is unreachable</t>
+          <t>The peering between as1r2 and 1.0.0.1 is not up.</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Checking that named is running on device `net`</t>
+          <t>Checking the routing table of as1r1</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -8941,14 +8771,14 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Device net not in the network scenario.</t>
+          <t>The routing table of as1r1 have the wrong number of routes: 6, expected: 8</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Checking that watchfrr is not running on device `net`</t>
+          <t>Checking the routing table of as1r2</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -8958,14 +8788,14 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Device net not in the network scenario.</t>
+          <t>The routing table of as1r2 have the wrong number of routes: 6, expected: 8</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Checking that named is running on device `root`</t>
+          <t>Checking the routing table of as2r1</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -8975,14 +8805,14 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Device root not in the network scenario.</t>
+          <t>The routing table of as2r1 have the wrong number of routes: 5, expected: 8</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Checking that watchfrr is not running on device `root`</t>
+          <t>Checking the routing table of as2r2</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -8992,14 +8822,14 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Device root not in the network scenario.</t>
+          <t>The routing table of as2r2 have the wrong number of routes: 4, expected: 8</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>as1r1 has bgp peer 1.0.0.2</t>
+          <t>Checking the routing table of as3r1</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -9009,14 +8839,14 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>The peering between as1r1 and 1.0.0.2 is not up.</t>
+          <t>The routing table of as3r1 have the wrong number of routes: 6, expected: 9</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>as1r2 has bgp peer 1.0.0.1</t>
+          <t>Checking the routing table of root</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -9026,14 +8856,14 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>The peering between as1r2 and 1.0.0.1 is not up.</t>
+          <t>The routing table of root have the wrong number of routes: 0, expected: 2</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Checking the routing table of as3r1</t>
+          <t>Checking the routing table of net</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -9043,14 +8873,14 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>The routing table of as3r1 is missing route 3.2.0.0/24</t>
+          <t>The routing table of net have the wrong number of routes: 0, expected: 2</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Checking the routing table of root</t>
+          <t>Checking the routing table of pc</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -9060,14 +8890,14 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>The routing table of root is missing route 0.0.0.0/0</t>
+          <t>The routing table of pc have the wrong number of routes: 0, expected: 2</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Checking the routing table of root</t>
+          <t>Checking the routing table of local</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -9077,14 +8907,14 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>The routing table of root is missing route 1.1.0.0/24</t>
+          <t>The routing table of local have the wrong number of routes: 0, expected: 2</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Checking the routing table of net</t>
+          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -9094,14 +8924,14 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>The routing table of net is missing route 0.0.0.0/0</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Checking the routing table of net</t>
+          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -9111,14 +8941,14 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>The routing table of net is missing route 2.1.0.0/24</t>
+          <t>Device `root` is not running.</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Checking the routing table of pc</t>
+          <t>Checking on `local` that `1.1.0.2` is the authority for domain `.`</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -9128,14 +8958,14 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>The routing table of pc is missing route 0.0.0.0/0</t>
+          <t>named not started in the startup file of `local`</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Checking the routing table of pc</t>
+          <t>Checking on `net` that `2.1.0.2` is the authority for domain `net`</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -9145,14 +8975,14 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>The routing table of pc is missing route 3.1.0.0/24</t>
+          <t>Device `net` is not running.</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Checking the routing table of local</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -9162,14 +8992,14 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>The routing table of local is missing route 0.0.0.0/0</t>
+          <t>`resolv.conf` file not found for device `as1r1`</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Checking the routing table of local</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -9179,14 +9009,14 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>The routing table of local is missing route 3.2.0.0/24</t>
+          <t>`resolv.conf` file not found for device `as1r2`</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -9196,14 +9026,14 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>`resolv.conf` file not found for device `as2r1`</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Checking on `root` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -9213,14 +9043,14 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Device `root` is not running.</t>
+          <t>`resolv.conf` file not found for device `as2r2`</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Checking on `local` that `1.1.0.2` is the authority for domain `.`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -9230,14 +9060,14 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>named not started in the startup file of `local`</t>
+          <t>`resolv.conf` file not found for device `as3r1`</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Checking on `net` that `2.1.0.2` is the authority for domain `net`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -9247,14 +9077,14 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Device `net` is not running.</t>
+          <t>`resolv.conf` file not found for device `as3r2`</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r1`</t>
+          <t>Checking that `3.2.0.2` is the local name server for device `pc`</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -9264,211 +9094,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>`resolv.conf` file not found for device `as1r1`</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as1r2`</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>`resolv.conf` file not found for device `as1r2`</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r1`</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>`resolv.conf` file not found for device `as2r1`</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as2r2`</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>`resolv.conf` file not found for device `as2r2`</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r1`</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>`resolv.conf` file not found for device `as3r1`</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `as3r2`</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>`resolv.conf` file not found for device `as3r2`</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>Checking that `3.2.0.2` is the local name server for device `pc`</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
           <t>The local name server for device `pc` has ip `3.2.0.2`</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as1r1`</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as1r2`</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as2r1`</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as2r2`</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as3r1`</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>Verifying `pc.net` reachable from device `as3r2`</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>ping: pc.net: Temporary failure in name resolution</t>
         </is>
       </c>
     </row>

</xml_diff>